<commit_message>
store price is 10 sale price is 10
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\27465\Desktop\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E971B1-722C-47D6-B85B-51DDCD33B5C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B665B5F-28AC-4821-8796-CCC30BD9E204}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="1485" windowWidth="15555" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4118" yWindow="1035" windowWidth="15554" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="city" sheetId="1" r:id="rId1"/>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -549,7 +549,7 @@
         <v>1000</v>
       </c>
       <c r="G3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -584,7 +584,7 @@
         <v>500</v>
       </c>
       <c r="G4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -619,7 +619,7 @@
         <v>700</v>
       </c>
       <c r="G5">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -654,7 +654,7 @@
         <v>800</v>
       </c>
       <c r="G6">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -689,7 +689,7 @@
         <v>300</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -724,7 +724,7 @@
         <v>900</v>
       </c>
       <c r="G8">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -759,7 +759,7 @@
         <v>700</v>
       </c>
       <c r="G9">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -794,7 +794,7 @@
         <v>400</v>
       </c>
       <c r="G10">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -829,7 +829,7 @@
         <v>300</v>
       </c>
       <c r="G11">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -864,7 +864,7 @@
         <v>700</v>
       </c>
       <c r="G12">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -899,7 +899,7 @@
         <v>500</v>
       </c>
       <c r="G13">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -934,7 +934,7 @@
         <v>132</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -969,7 +969,7 @@
         <v>341</v>
       </c>
       <c r="G15">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1004,7 +1004,7 @@
         <v>3214</v>
       </c>
       <c r="G16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1039,7 +1039,7 @@
         <v>312</v>
       </c>
       <c r="G17">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1074,7 +1074,7 @@
         <v>4113</v>
       </c>
       <c r="G18">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1144,7 +1144,7 @@
         <v>1234</v>
       </c>
       <c r="G20">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1179,7 +1179,7 @@
         <v>1341</v>
       </c>
       <c r="G21">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1214,7 +1214,7 @@
         <v>2314</v>
       </c>
       <c r="G22">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1249,7 +1249,7 @@
         <v>3511</v>
       </c>
       <c r="G23">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1284,7 +1284,7 @@
         <v>1334</v>
       </c>
       <c r="G24">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1319,7 +1319,7 @@
         <v>1234</v>
       </c>
       <c r="G25">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1354,7 +1354,7 @@
         <v>1234</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1389,7 +1389,7 @@
         <v>5243</v>
       </c>
       <c r="G27">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1424,7 +1424,7 @@
         <v>3141</v>
       </c>
       <c r="G28">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -1459,7 +1459,7 @@
         <v>1234</v>
       </c>
       <c r="G29">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -1494,7 +1494,7 @@
         <v>1234</v>
       </c>
       <c r="G30">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -1529,7 +1529,7 @@
         <v>5234</v>
       </c>
       <c r="G31">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1564,7 +1564,7 @@
         <v>4513</v>
       </c>
       <c r="G32">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -1599,7 +1599,7 @@
         <v>1345</v>
       </c>
       <c r="G33">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -1669,7 +1669,7 @@
         <v>345</v>
       </c>
       <c r="G35">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -1704,7 +1704,7 @@
         <v>634</v>
       </c>
       <c r="G36">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -1739,7 +1739,7 @@
         <v>2523</v>
       </c>
       <c r="G37">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -1774,7 +1774,7 @@
         <v>2345</v>
       </c>
       <c r="G38">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -1809,7 +1809,7 @@
         <v>3652</v>
       </c>
       <c r="G39">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -1844,7 +1844,7 @@
         <v>2346</v>
       </c>
       <c r="G40">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -1879,7 +1879,7 @@
         <v>4325</v>
       </c>
       <c r="G41">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -1914,7 +1914,7 @@
         <v>365</v>
       </c>
       <c r="G42">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -1949,7 +1949,7 @@
         <v>6345</v>
       </c>
       <c r="G43">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -1984,7 +1984,7 @@
         <v>4562</v>
       </c>
       <c r="G44">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -2019,7 +2019,7 @@
         <v>5252</v>
       </c>
       <c r="G45">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -2089,7 +2089,7 @@
         <v>2534</v>
       </c>
       <c r="G47">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -2124,7 +2124,7 @@
         <v>3643</v>
       </c>
       <c r="G48">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -2159,7 +2159,7 @@
         <v>2345</v>
       </c>
       <c r="G49">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H49">
         <v>0</v>

</xml_diff>